<commit_message>
replaced the fieldname of all primary keys to 'id' so can simplify node.js coding
</commit_message>
<xml_diff>
--- a/demo_data/demo.xlsx
+++ b/demo_data/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseulloa/Developer/utilities-database-tools/demo_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E1DE0F-BC82-2C47-892B-E02BAD632C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EB80B7-F132-CF45-AE65-3BF919EBF918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="840" windowWidth="25800" windowHeight="16940" activeTab="5" xr2:uid="{D5A4ABC1-F07C-5E41-9CF5-2934409BBBCB}"/>
+    <workbookView xWindow="4680" yWindow="840" windowWidth="25800" windowHeight="16940" activeTab="5" xr2:uid="{D5A4ABC1-F07C-5E41-9CF5-2934409BBBCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="6" r:id="rId1"/>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>ProviderName</t>
-  </si>
-  <si>
-    <t>BillID</t>
   </si>
   <si>
     <t>MeterID</t>
@@ -254,6 +251,9 @@
   </si>
   <si>
     <t>4623794</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -631,45 +631,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDBB9C7-577C-3A4B-9409-C62926994DD2}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>37</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>40</v>
-      </c>
-      <c r="K1" t="s">
-        <v>41</v>
       </c>
       <c r="L1" t="s">
         <v>3</v>
@@ -683,31 +681,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>46</v>
-      </c>
-      <c r="D2" t="s">
-        <v>47</v>
       </c>
       <c r="E2">
         <v>3760</v>
       </c>
       <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
         <v>48</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>49</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>50</v>
       </c>
-      <c r="I2" t="s">
-        <v>51</v>
-      </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K2">
         <v>5475231</v>
@@ -728,9 +726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B6B2E9-B500-384C-A3D7-8831347B1FAA}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -741,7 +737,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -761,10 +757,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1">
         <v>45292</v>
@@ -778,10 +774,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1">
         <v>45292</v>
@@ -795,10 +791,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1">
         <v>45292</v>
@@ -812,10 +808,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1">
         <v>45292</v>
@@ -829,7 +825,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1">
         <v>45292</v>
@@ -843,10 +839,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1">
         <v>45292</v>
@@ -860,10 +856,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1">
         <v>45292</v>
@@ -881,9 +877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352205B7-8FEB-1A44-9AEF-084F7BD23C04}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -894,7 +888,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -917,7 +911,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1">
         <v>43678</v>
@@ -935,7 +929,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="1">
         <v>43678</v>
@@ -953,7 +947,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="1">
         <v>43678</v>
@@ -971,7 +965,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="1">
         <v>43678</v>
@@ -989,7 +983,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="1">
         <v>43678</v>
@@ -1007,7 +1001,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="1">
         <v>43678</v>
@@ -1025,7 +1019,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="1">
         <v>43678</v>
@@ -1047,9 +1041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5AD8BA3-D9F4-DF40-8DF0-FC7CECBA003D}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1058,13 +1050,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -1081,7 +1073,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D2" s="1">
         <v>43466</v>
@@ -1098,7 +1090,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="1">
         <v>43466</v>
@@ -1115,7 +1107,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="1">
         <v>43466</v>
@@ -1132,7 +1124,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="1">
         <v>43466</v>
@@ -1163,7 +1155,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="1">
         <v>43466</v>
@@ -1180,7 +1172,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" s="1">
         <v>43466</v>
@@ -1198,9 +1190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E458880D-D775-7B47-83F8-95DB757DD44F}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1210,10 +1200,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -1222,10 +1212,10 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1245,7 +1235,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1265,7 +1255,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1285,7 +1275,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1305,7 +1295,7 @@
         <v>4</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1325,7 +1315,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1345,7 +1335,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1365,7 +1355,7 @@
         <v>7</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1378,7 +1368,7 @@
   <dimension ref="A1:L336"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1396,34 +1386,34 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
       <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
         <v>43</v>
-      </c>
-      <c r="J1" t="s">
-        <v>44</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
@@ -1455,7 +1445,7 @@
         <v>43704</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I2" s="1">
         <v>43687</v>
@@ -1493,7 +1483,7 @@
         <v>43737</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I3" s="1">
         <v>43664</v>
@@ -1531,7 +1521,7 @@
         <v>43709</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I4" s="1">
         <v>43672</v>
@@ -1569,7 +1559,7 @@
         <v>43720</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I5" s="1">
         <v>43677</v>
@@ -1607,7 +1597,7 @@
         <v>43716</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I6" s="1">
         <v>43678</v>
@@ -1645,7 +1635,7 @@
         <v>43735</v>
       </c>
       <c r="H7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I7" s="1">
         <v>43723</v>
@@ -1683,7 +1673,7 @@
         <v>43737</v>
       </c>
       <c r="H8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I8" s="1">
         <v>43693</v>
@@ -1721,7 +1711,7 @@
         <v>43745</v>
       </c>
       <c r="H9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I9" s="1">
         <v>43704</v>
@@ -1759,7 +1749,7 @@
         <v>43745</v>
       </c>
       <c r="H10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I10" s="1">
         <v>43709</v>
@@ -1797,7 +1787,7 @@
         <v>43762</v>
       </c>
       <c r="H11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I11" s="1">
         <v>43753</v>
@@ -1835,7 +1825,7 @@
         <v>43753</v>
       </c>
       <c r="H12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I12" s="1">
         <v>43707</v>
@@ -1873,7 +1863,7 @@
         <v>43777</v>
       </c>
       <c r="H13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I13" s="1">
         <v>43721</v>
@@ -1911,7 +1901,7 @@
         <v>43777</v>
       </c>
       <c r="H14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I14" s="1">
         <v>43735</v>
@@ -1949,7 +1939,7 @@
         <v>43777</v>
       </c>
       <c r="H15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I15" s="1">
         <v>43739</v>
@@ -1987,7 +1977,7 @@
         <v>43787</v>
       </c>
       <c r="H16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I16" s="1">
         <v>43739</v>
@@ -2025,7 +2015,7 @@
         <v>43787</v>
       </c>
       <c r="H17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I17" s="1">
         <v>43784</v>
@@ -2063,7 +2053,7 @@
         <v>43797</v>
       </c>
       <c r="H18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I18" s="1">
         <v>43755</v>
@@ -2101,7 +2091,7 @@
         <v>43803</v>
       </c>
       <c r="H19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I19" s="1">
         <v>43767</v>
@@ -2139,7 +2129,7 @@
         <v>43808</v>
       </c>
       <c r="H20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I20" s="1">
         <v>43770</v>
@@ -2177,7 +2167,7 @@
         <v>43818</v>
       </c>
       <c r="H21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I21" s="1">
         <v>43814</v>
@@ -2215,7 +2205,7 @@
         <v>43818</v>
       </c>
       <c r="H22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I22" s="1">
         <v>43769</v>
@@ -2253,7 +2243,7 @@
         <v>43829</v>
       </c>
       <c r="H23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I23" s="1">
         <v>43784</v>
@@ -2291,7 +2281,7 @@
         <v>43844</v>
       </c>
       <c r="H24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I24" s="1">
         <v>43795</v>
@@ -2329,7 +2319,7 @@
         <v>43841</v>
       </c>
       <c r="H25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I25" s="1">
         <v>43800</v>
@@ -2367,7 +2357,7 @@
         <v>43844</v>
       </c>
       <c r="H26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I26" s="1">
         <v>43798</v>
@@ -2405,7 +2395,7 @@
         <v>43858</v>
       </c>
       <c r="H27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I27" s="1">
         <v>43845</v>
@@ -2443,7 +2433,7 @@
         <v>43858</v>
       </c>
       <c r="H28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I28" s="1">
         <v>43815</v>
@@ -2481,7 +2471,7 @@
         <v>43872</v>
       </c>
       <c r="H29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I29" s="1">
         <v>43824</v>
@@ -2519,7 +2509,7 @@
         <v>43872</v>
       </c>
       <c r="H30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I30" s="1">
         <v>43831</v>
@@ -2557,7 +2547,7 @@
         <v>43879</v>
       </c>
       <c r="H31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I31" s="1">
         <v>43829</v>
@@ -2595,7 +2585,7 @@
         <v>43885</v>
       </c>
       <c r="H32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I32" s="1">
         <v>43876</v>
@@ -2633,7 +2623,7 @@
         <v>43885</v>
       </c>
       <c r="H33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I33" s="1">
         <v>43847</v>
@@ -2671,7 +2661,7 @@
         <v>43892</v>
       </c>
       <c r="H34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I34" s="1">
         <v>43855</v>
@@ -2709,7 +2699,7 @@
         <v>43900</v>
       </c>
       <c r="H35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I35" s="1">
         <v>43862</v>
@@ -2747,7 +2737,7 @@
         <v>43902</v>
       </c>
       <c r="H36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I36" s="1">
         <v>43860</v>
@@ -2785,7 +2775,7 @@
         <v>43917</v>
       </c>
       <c r="H37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I37" s="1">
         <v>43905</v>
@@ -2823,7 +2813,7 @@
         <v>43927</v>
       </c>
       <c r="H38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I38" s="1">
         <v>43875</v>
@@ -2861,7 +2851,7 @@
         <v>43927</v>
       </c>
       <c r="H39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I39" s="1">
         <v>43886</v>
@@ -2899,7 +2889,7 @@
         <v>43933</v>
       </c>
       <c r="H40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I40" s="1">
         <v>43891</v>
@@ -2937,7 +2927,7 @@
         <v>43933</v>
       </c>
       <c r="H41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I41" s="1">
         <v>43892</v>
@@ -2975,7 +2965,7 @@
         <v>43933</v>
       </c>
       <c r="H42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I42" s="1">
         <v>43936</v>
@@ -3013,7 +3003,7 @@
         <v>43984</v>
       </c>
       <c r="H43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I43" s="1">
         <v>43907</v>
@@ -3051,7 +3041,7 @@
         <v>43957</v>
       </c>
       <c r="H44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I44" s="1">
         <v>43916</v>
@@ -3089,7 +3079,7 @@
         <v>43963</v>
       </c>
       <c r="H45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I45" s="1">
         <v>43922</v>
@@ -3127,7 +3117,7 @@
         <v>43963</v>
       </c>
       <c r="H46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I46" s="1">
         <v>43921</v>
@@ -3165,7 +3155,7 @@
         <v>43963</v>
       </c>
       <c r="H47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I47" s="1">
         <v>43966</v>
@@ -3203,7 +3193,7 @@
         <v>43984</v>
       </c>
       <c r="H48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I48" s="1">
         <v>43938</v>
@@ -3241,7 +3231,7 @@
         <v>43997</v>
       </c>
       <c r="H49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I49" s="1">
         <v>43949</v>
@@ -3279,7 +3269,7 @@
         <v>43997</v>
       </c>
       <c r="H50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I50" s="1">
         <v>43952</v>
@@ -3317,7 +3307,7 @@
         <v>43997</v>
       </c>
       <c r="H51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I51" s="1">
         <v>43950</v>
@@ -3355,7 +3345,7 @@
         <v>43997</v>
       </c>
       <c r="H52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I52" s="1">
         <v>43997</v>
@@ -3393,7 +3383,7 @@
         <v>44019</v>
       </c>
       <c r="H53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I53" s="1">
         <v>43966</v>
@@ -3431,7 +3421,7 @@
         <v>44026</v>
       </c>
       <c r="H54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I54" s="1">
         <v>43978</v>
@@ -3469,7 +3459,7 @@
         <v>44019</v>
       </c>
       <c r="H55" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I55" s="1">
         <v>43983</v>
@@ -3507,7 +3497,7 @@
         <v>44026</v>
       </c>
       <c r="H56" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I56" s="1">
         <v>43981</v>
@@ -3545,7 +3535,7 @@
         <v>44042</v>
       </c>
       <c r="H57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I57" s="1">
         <v>44027</v>
@@ -3583,7 +3573,7 @@
         <v>44053</v>
       </c>
       <c r="H58" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I58" s="1">
         <v>43998</v>
@@ -3621,7 +3611,7 @@
         <v>44053</v>
       </c>
       <c r="H59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I59" s="1">
         <v>44007</v>
@@ -3659,7 +3649,7 @@
         <v>44053</v>
       </c>
       <c r="H60" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I60" s="1">
         <v>44013</v>
@@ -3697,7 +3687,7 @@
         <v>44053</v>
       </c>
       <c r="H61" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I61" s="1">
         <v>44013</v>
@@ -3735,7 +3725,7 @@
         <v>44073</v>
       </c>
       <c r="H62" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I62" s="1">
         <v>44058</v>
@@ -3773,7 +3763,7 @@
         <v>44080</v>
       </c>
       <c r="H63" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I63" s="1">
         <v>44029</v>
@@ -3811,7 +3801,7 @@
         <v>44080</v>
       </c>
       <c r="H64" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I64" s="1">
         <v>44040</v>
@@ -3849,7 +3839,7 @@
         <v>44080</v>
       </c>
       <c r="H65" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I65" s="1">
         <v>44044</v>
@@ -3887,7 +3877,7 @@
         <v>44102</v>
       </c>
       <c r="H66" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I66" s="1">
         <v>44043</v>
@@ -3925,7 +3915,7 @@
         <v>44103</v>
       </c>
       <c r="H67" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I67" s="1">
         <v>44089</v>
@@ -3963,7 +3953,7 @@
         <v>44116</v>
       </c>
       <c r="H68" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I68" s="1">
         <v>44057</v>
@@ -4001,7 +3991,7 @@
         <v>44116</v>
       </c>
       <c r="H69" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I69" s="1">
         <v>44070</v>
@@ -4039,7 +4029,7 @@
         <v>44116</v>
       </c>
       <c r="H70" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I70" s="1">
         <v>44075</v>
@@ -4077,7 +4067,7 @@
         <v>44116</v>
       </c>
       <c r="H71" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I71" s="1">
         <v>44074</v>
@@ -4115,7 +4105,7 @@
         <v>44134</v>
       </c>
       <c r="H72" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I72" s="1">
         <v>44119</v>
@@ -4153,7 +4143,7 @@
         <v>44160</v>
       </c>
       <c r="H73" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I73" s="1">
         <v>44120</v>
@@ -4191,7 +4181,7 @@
         <v>44143</v>
       </c>
       <c r="H74" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I74" s="1">
         <v>44089</v>
@@ -4229,7 +4219,7 @@
         <v>44143</v>
       </c>
       <c r="H75" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I75" s="1">
         <v>44100</v>
@@ -4267,7 +4257,7 @@
         <v>44143</v>
       </c>
       <c r="H76" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I76" s="1">
         <v>44105</v>
@@ -4305,7 +4295,7 @@
         <v>44143</v>
       </c>
       <c r="H77" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I77" s="1">
         <v>44104</v>
@@ -4343,7 +4333,7 @@
         <v>44165</v>
       </c>
       <c r="H78" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I78" s="1">
         <v>44150</v>
@@ -4381,7 +4371,7 @@
         <v>44173</v>
       </c>
       <c r="H79" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I79" s="1">
         <v>44132</v>
@@ -4419,7 +4409,7 @@
         <v>44173</v>
       </c>
       <c r="H80" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I80" s="1">
         <v>44136</v>
@@ -4457,7 +4447,7 @@
         <v>44193</v>
       </c>
       <c r="H81" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I81" s="1">
         <v>44134</v>
@@ -4495,7 +4485,7 @@
         <v>44193</v>
       </c>
       <c r="H82" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I82" s="1">
         <v>44180</v>
@@ -4533,7 +4523,7 @@
         <v>44193</v>
       </c>
       <c r="H83" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I83" s="1">
         <v>44151</v>
@@ -4571,7 +4561,7 @@
         <v>44205</v>
       </c>
       <c r="H84" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I84" s="1">
         <v>44161</v>
@@ -4609,7 +4599,7 @@
         <v>44205</v>
       </c>
       <c r="H85" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I85" s="1">
         <v>44166</v>
@@ -4647,7 +4637,7 @@
         <v>44205</v>
       </c>
       <c r="H86" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I86" s="1">
         <v>44165</v>
@@ -4685,7 +4675,7 @@
         <v>44226</v>
       </c>
       <c r="H87" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I87" s="1">
         <v>44211</v>
@@ -4723,7 +4713,7 @@
         <v>44226</v>
       </c>
       <c r="H88" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I88" s="1">
         <v>44181</v>
@@ -4761,7 +4751,7 @@
         <v>44251</v>
       </c>
       <c r="H89" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I89" s="1">
         <v>44190</v>
@@ -4799,7 +4789,7 @@
         <v>44234</v>
       </c>
       <c r="H90" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I90" s="1">
         <v>44197</v>
@@ -4837,7 +4827,7 @@
         <v>44253</v>
       </c>
       <c r="H91" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I91" s="1">
         <v>44195</v>
@@ -4875,7 +4865,7 @@
         <v>44251</v>
       </c>
       <c r="H92" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I92" s="1">
         <v>44242</v>
@@ -4913,7 +4903,7 @@
         <v>44265</v>
       </c>
       <c r="H93" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I93" s="1">
         <v>44215</v>
@@ -4951,7 +4941,7 @@
         <v>44265</v>
       </c>
       <c r="H94" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I94" s="1">
         <v>44215</v>
@@ -4989,7 +4979,7 @@
         <v>44265</v>
       </c>
       <c r="H95" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I95" s="1">
         <v>44223</v>
@@ -5027,7 +5017,7 @@
         <v>44265</v>
       </c>
       <c r="H96" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I96" s="1">
         <v>44228</v>
@@ -5065,7 +5055,7 @@
         <v>44265</v>
       </c>
       <c r="H97" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I97" s="1">
         <v>44224</v>
@@ -5103,7 +5093,7 @@
         <v>44265</v>
       </c>
       <c r="H98" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I98" s="1">
         <v>44265</v>
@@ -5141,7 +5131,7 @@
         <v>44296</v>
       </c>
       <c r="H99" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I99" s="1">
         <v>44246</v>
@@ -5179,7 +5169,7 @@
         <v>44302</v>
       </c>
       <c r="H100" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I100" s="1">
         <v>44243</v>
@@ -5217,7 +5207,7 @@
         <v>44302</v>
       </c>
       <c r="H101" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I101" s="1">
         <v>44251</v>
@@ -5255,7 +5245,7 @@
         <v>44298</v>
       </c>
       <c r="H102" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I102" s="1">
         <v>44256</v>
@@ -5293,7 +5283,7 @@
         <v>44302</v>
       </c>
       <c r="H103" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I103" s="1">
         <v>44256</v>
@@ -5331,7 +5321,7 @@
         <v>44302</v>
       </c>
       <c r="H104" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I104" s="1">
         <v>44301</v>
@@ -5369,7 +5359,7 @@
         <v>44329</v>
       </c>
       <c r="H105" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I105" s="1">
         <v>44274</v>
@@ -5407,7 +5397,7 @@
         <v>44332</v>
       </c>
       <c r="H106" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I106" s="1">
         <v>44272</v>
@@ -5445,7 +5435,7 @@
         <v>44332</v>
       </c>
       <c r="H107" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I107" s="1">
         <v>44281</v>
@@ -5483,7 +5473,7 @@
         <v>44332</v>
       </c>
       <c r="H108" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I108" s="1">
         <v>44287</v>
@@ -5521,7 +5511,7 @@
         <v>44332</v>
       </c>
       <c r="H109" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I109" s="1">
         <v>44285</v>
@@ -5559,7 +5549,7 @@
         <v>44332</v>
       </c>
       <c r="H110" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I110" s="1">
         <v>44331</v>
@@ -5597,7 +5587,7 @@
         <v>44356</v>
       </c>
       <c r="H111" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I111" s="1">
         <v>44302</v>
@@ -5635,7 +5625,7 @@
         <v>44355</v>
       </c>
       <c r="H112" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I112" s="1">
         <v>44305</v>
@@ -5673,7 +5663,7 @@
         <v>44356</v>
       </c>
       <c r="H113" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I113" s="1">
         <v>44314</v>
@@ -5711,7 +5701,7 @@
         <v>44356</v>
       </c>
       <c r="H114" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I114" s="1">
         <v>44317</v>
@@ -5749,7 +5739,7 @@
         <v>44368</v>
       </c>
       <c r="H115" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I115" s="1">
         <v>44315</v>
@@ -5787,7 +5777,7 @@
         <v>44368</v>
       </c>
       <c r="H116" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I116" s="1">
         <v>44362</v>
@@ -5825,7 +5815,7 @@
         <v>44368</v>
       </c>
       <c r="H117" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I117" s="1">
         <v>44330</v>
@@ -5863,7 +5853,7 @@
         <v>44385</v>
       </c>
       <c r="H118" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I118" s="1">
         <v>44335</v>
@@ -5901,7 +5891,7 @@
         <v>44385</v>
       </c>
       <c r="H119" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I119" s="1">
         <v>44343</v>
@@ -5939,7 +5929,7 @@
         <v>44385</v>
       </c>
       <c r="H120" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I120" s="1">
         <v>44348</v>
@@ -5977,7 +5967,7 @@
         <v>44406</v>
       </c>
       <c r="H121" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I121" s="1">
         <v>44347</v>
@@ -6015,7 +6005,7 @@
         <v>44406</v>
       </c>
       <c r="H122" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I122" s="1">
         <v>44387</v>
@@ -6053,7 +6043,7 @@
         <v>44406</v>
       </c>
       <c r="H123" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I123" s="1">
         <v>44366</v>
@@ -6091,7 +6081,7 @@
         <v>44406</v>
       </c>
       <c r="H124" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I124" s="1">
         <v>44361</v>
@@ -6129,7 +6119,7 @@
         <v>44422</v>
       </c>
       <c r="H125" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I125" s="1">
         <v>44373</v>
@@ -6167,7 +6157,7 @@
         <v>44422</v>
       </c>
       <c r="H126" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I126" s="1">
         <v>44378</v>
@@ -6205,7 +6195,7 @@
         <v>44422</v>
       </c>
       <c r="H127" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I127" s="1">
         <v>44377</v>
@@ -6243,7 +6233,7 @@
         <v>44422</v>
       </c>
       <c r="H128" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I128" s="1">
         <v>44418</v>
@@ -6281,7 +6271,7 @@
         <v>44447</v>
       </c>
       <c r="H129" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I129" s="1">
         <v>44396</v>
@@ -6319,7 +6309,7 @@
         <v>44452</v>
       </c>
       <c r="H130" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I130" s="1">
         <v>44392</v>
@@ -6357,7 +6347,7 @@
         <v>44452</v>
       </c>
       <c r="H131" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I131" s="1">
         <v>44405</v>
@@ -6395,7 +6385,7 @@
         <v>44449</v>
       </c>
       <c r="H132" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I132" s="1">
         <v>44409</v>
@@ -6433,7 +6423,7 @@
         <v>44468</v>
       </c>
       <c r="H133" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I133" s="1">
         <v>44407</v>
@@ -6471,7 +6461,7 @@
         <v>44468</v>
       </c>
       <c r="H134" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I134" s="1">
         <v>44449</v>
@@ -6509,7 +6499,7 @@
         <v>44477</v>
       </c>
       <c r="H135" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I135" s="1">
         <v>44427</v>
@@ -6547,7 +6537,7 @@
         <v>44484</v>
       </c>
       <c r="H136" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I136" s="1">
         <v>44425</v>
@@ -6585,7 +6575,7 @@
         <v>44484</v>
       </c>
       <c r="H137" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I137" s="1">
         <v>44435</v>
@@ -6623,7 +6613,7 @@
         <v>44484</v>
       </c>
       <c r="H138" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I138" s="1">
         <v>44440</v>
@@ -6661,7 +6651,7 @@
         <v>44484</v>
       </c>
       <c r="H139" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I139" s="1">
         <v>44439</v>
@@ -6699,7 +6689,7 @@
         <v>44484</v>
       </c>
       <c r="H140" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I140" s="1">
         <v>44479</v>
@@ -6737,7 +6727,7 @@
         <v>44508</v>
       </c>
       <c r="H141" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I141" s="1">
         <v>44458</v>
@@ -6775,7 +6765,7 @@
         <v>44510</v>
       </c>
       <c r="H142" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I142" s="1">
         <v>44455</v>
@@ -6813,7 +6803,7 @@
         <v>44512</v>
       </c>
       <c r="H143" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I143" s="1">
         <v>44467</v>
@@ -6851,7 +6841,7 @@
         <v>44510</v>
       </c>
       <c r="H144" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I144" s="1">
         <v>44470</v>
@@ -6889,7 +6879,7 @@
         <v>44510</v>
       </c>
       <c r="H145" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I145" s="1">
         <v>44469</v>
@@ -6927,7 +6917,7 @@
         <v>44529</v>
       </c>
       <c r="H146" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I146" s="1">
         <v>44510</v>
@@ -6965,7 +6955,7 @@
         <v>44539</v>
       </c>
       <c r="H147" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I147" s="1">
         <v>44488</v>
@@ -7003,7 +6993,7 @@
         <v>44549</v>
       </c>
       <c r="H148" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I148" s="1">
         <v>44488</v>
@@ -7041,7 +7031,7 @@
         <v>44544</v>
       </c>
       <c r="H149" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I149" s="1">
         <v>44496</v>
@@ -7079,7 +7069,7 @@
         <v>44543</v>
       </c>
       <c r="H150" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I150" s="1">
         <v>44501</v>
@@ -7117,7 +7107,7 @@
         <v>44549</v>
       </c>
       <c r="H151" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I151" s="1">
         <v>44499</v>
@@ -7155,7 +7145,7 @@
         <v>44549</v>
       </c>
       <c r="H152" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I152" s="1">
         <v>44540</v>
@@ -7193,7 +7183,7 @@
         <v>44569</v>
       </c>
       <c r="H153" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I153" s="1">
         <v>44519</v>
@@ -7231,7 +7221,7 @@
         <v>44570</v>
       </c>
       <c r="H154" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I154" s="1">
         <v>44517</v>
@@ -7269,7 +7259,7 @@
         <v>44574</v>
       </c>
       <c r="H155" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I155" s="1">
         <v>44526</v>
@@ -7307,7 +7297,7 @@
         <v>44570</v>
       </c>
       <c r="H156" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I156" s="1">
         <v>44531</v>
@@ -7345,7 +7335,7 @@
         <v>44591</v>
       </c>
       <c r="H157" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I157" s="1">
         <v>44531</v>
@@ -7383,7 +7373,7 @@
         <v>44591</v>
       </c>
       <c r="H158" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I158" s="1">
         <v>44571</v>
@@ -7421,7 +7411,7 @@
         <v>44600</v>
       </c>
       <c r="H159" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I159" s="1">
         <v>44549</v>
@@ -7459,7 +7449,7 @@
         <v>44591</v>
       </c>
       <c r="H160" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I160" s="1">
         <v>44546</v>
@@ -7497,7 +7487,7 @@
         <v>44603</v>
       </c>
       <c r="H161" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I161" s="1">
         <v>44558</v>
@@ -7535,7 +7525,7 @@
         <v>44612</v>
       </c>
       <c r="H162" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I162" s="1">
         <v>44562</v>
@@ -7573,7 +7563,7 @@
         <v>44612</v>
       </c>
       <c r="H163" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I163" s="1">
         <v>44559</v>
@@ -7611,7 +7601,7 @@
         <v>44612</v>
       </c>
       <c r="H164" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I164" s="1">
         <v>44602</v>
@@ -7649,7 +7639,7 @@
         <v>44631</v>
       </c>
       <c r="H165" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I165" s="1">
         <v>44580</v>
@@ -7687,7 +7677,7 @@
         <v>44631</v>
       </c>
       <c r="H166" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I166" s="1">
         <v>44578</v>
@@ -7725,7 +7715,7 @@
         <v>44631</v>
       </c>
       <c r="H167" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I167" s="1">
         <v>44588</v>
@@ -7763,7 +7753,7 @@
         <v>44631</v>
       </c>
       <c r="H168" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I168" s="1">
         <v>44593</v>
@@ -7801,7 +7791,7 @@
         <v>44662</v>
       </c>
       <c r="H169" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I169" s="1">
         <v>44589</v>
@@ -7839,7 +7829,7 @@
         <v>44650</v>
       </c>
       <c r="H170" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I170" s="1">
         <v>44630</v>
@@ -7877,7 +7867,7 @@
         <v>44659</v>
       </c>
       <c r="H171" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I171" s="1">
         <v>44611</v>
@@ -7915,7 +7905,7 @@
         <v>44662</v>
       </c>
       <c r="H172" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I172" s="1">
         <v>44609</v>
@@ -7953,7 +7943,7 @@
         <v>44663</v>
       </c>
       <c r="H173" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I173" s="1">
         <v>44616</v>
@@ -7991,7 +7981,7 @@
         <v>44662</v>
       </c>
       <c r="H174" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I174" s="1">
         <v>44621</v>
@@ -8029,7 +8019,7 @@
         <v>44662</v>
       </c>
       <c r="H175" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I175" s="1">
         <v>44620</v>
@@ -8067,7 +8057,7 @@
         <v>44690</v>
       </c>
       <c r="H176" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I176" s="1">
         <v>44639</v>
@@ -8105,7 +8095,7 @@
         <v>44692</v>
       </c>
       <c r="H177" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I177" s="1">
         <v>44637</v>
@@ -8143,7 +8133,7 @@
         <v>44693</v>
       </c>
       <c r="H178" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I178" s="1">
         <v>44646</v>
@@ -8181,7 +8171,7 @@
         <v>44691</v>
       </c>
       <c r="H179" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I179" s="1">
         <v>44652</v>
@@ -8219,7 +8209,7 @@
         <v>44692</v>
       </c>
       <c r="H180" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I180" s="1">
         <v>44658</v>
@@ -8257,7 +8247,7 @@
         <v>44712</v>
       </c>
       <c r="H181" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I181" s="1">
         <v>44650</v>
@@ -8295,7 +8285,7 @@
         <v>44720</v>
       </c>
       <c r="H182" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I182" s="1">
         <v>44670</v>
@@ -8333,7 +8323,7 @@
         <v>44724</v>
       </c>
       <c r="H183" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I183" s="1">
         <v>44669</v>
@@ -8371,7 +8361,7 @@
         <v>44724</v>
       </c>
       <c r="H184" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I184" s="1">
         <v>44678</v>
@@ -8409,7 +8399,7 @@
         <v>44724</v>
       </c>
       <c r="H185" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I185" s="1">
         <v>44682</v>
@@ -8447,7 +8437,7 @@
         <v>44734</v>
       </c>
       <c r="H186" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I186" s="1">
         <v>44682</v>
@@ -8485,7 +8475,7 @@
         <v>44724</v>
       </c>
       <c r="H187" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I187" s="1">
         <v>44681</v>
@@ -8523,7 +8513,7 @@
         <v>44750</v>
       </c>
       <c r="H188" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I188" s="1">
         <v>44700</v>
@@ -8561,7 +8551,7 @@
         <v>44752</v>
       </c>
       <c r="H189" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I189" s="1">
         <v>44700</v>
@@ -8599,7 +8589,7 @@
         <v>44752</v>
       </c>
       <c r="H190" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I190" s="1">
         <v>44708</v>
@@ -8637,7 +8627,7 @@
         <v>44752</v>
       </c>
       <c r="H191" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I191" s="1">
         <v>44713</v>
@@ -8675,7 +8665,7 @@
         <v>44763</v>
       </c>
       <c r="H192" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I192" s="1">
         <v>44713</v>
@@ -8713,7 +8703,7 @@
         <v>44752</v>
       </c>
       <c r="H193" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I193" s="1">
         <v>44713</v>
@@ -8751,7 +8741,7 @@
         <v>44781</v>
       </c>
       <c r="H194" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I194" s="1">
         <v>44731</v>
@@ -8789,7 +8779,7 @@
         <v>44796</v>
       </c>
       <c r="H195" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I195" s="1">
         <v>44728</v>
@@ -8827,7 +8817,7 @@
         <v>44796</v>
       </c>
       <c r="H196" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I196" s="1">
         <v>44738</v>
@@ -8865,7 +8855,7 @@
         <v>44794</v>
       </c>
       <c r="H197" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I197" s="1">
         <v>44743</v>
@@ -8903,7 +8893,7 @@
         <v>44789</v>
       </c>
       <c r="H198" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I198" s="1">
         <v>44743</v>
@@ -8941,7 +8931,7 @@
         <v>44796</v>
       </c>
       <c r="H199" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I199" s="1">
         <v>44743</v>
@@ -8979,7 +8969,7 @@
         <v>44812</v>
       </c>
       <c r="H200" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I200" s="1">
         <v>44761</v>
@@ -9017,7 +9007,7 @@
         <v>44822</v>
       </c>
       <c r="H201" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I201" s="1">
         <v>44760</v>
@@ -9055,7 +9045,7 @@
         <v>44844</v>
       </c>
       <c r="H202" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I202" s="1">
         <v>44769</v>
@@ -9093,7 +9083,7 @@
         <v>44814</v>
       </c>
       <c r="H203" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I203" s="1">
         <v>44774</v>
@@ -9131,7 +9121,7 @@
         <v>44825</v>
       </c>
       <c r="H204" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I204" s="1">
         <v>44774</v>
@@ -9169,7 +9159,7 @@
         <v>44844</v>
       </c>
       <c r="H205" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I205" s="1">
         <v>44774</v>
@@ -9207,7 +9197,7 @@
         <v>44843</v>
       </c>
       <c r="H206" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I206" s="1">
         <v>44792</v>
@@ -9245,7 +9235,7 @@
         <v>44844</v>
       </c>
       <c r="H207" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I207" s="1">
         <v>44791</v>
@@ -9283,7 +9273,7 @@
         <v>44844</v>
       </c>
       <c r="H208" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I208" s="1">
         <v>44800</v>
@@ -9321,7 +9311,7 @@
         <v>44855</v>
       </c>
       <c r="H209" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I209" s="1">
         <v>44805</v>
@@ -9359,7 +9349,7 @@
         <v>44844</v>
       </c>
       <c r="H210" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I210" s="1">
         <v>44805</v>
@@ -9397,7 +9387,7 @@
         <v>44844</v>
       </c>
       <c r="H211" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I211" s="1">
         <v>44804</v>
@@ -9435,7 +9425,7 @@
         <v>44873</v>
       </c>
       <c r="H212" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I212" s="1">
         <v>44823</v>
@@ -9473,7 +9463,7 @@
         <v>44899</v>
       </c>
       <c r="H213" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I213" s="1">
         <v>44818</v>
@@ -9511,7 +9501,7 @@
         <v>44899</v>
       </c>
       <c r="H214" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I214" s="1">
         <v>44832</v>
@@ -9549,7 +9539,7 @@
         <v>44877</v>
       </c>
       <c r="H215" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I215" s="1">
         <v>44835</v>
@@ -9587,7 +9577,7 @@
         <v>44886</v>
       </c>
       <c r="H216" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I216" s="1">
         <v>44835</v>
@@ -9625,7 +9615,7 @@
         <v>44899</v>
       </c>
       <c r="H217" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I217" s="1">
         <v>44835</v>
@@ -9663,7 +9653,7 @@
         <v>44904</v>
       </c>
       <c r="H218" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I218" s="1">
         <v>44853</v>
@@ -9701,7 +9691,7 @@
         <v>44899</v>
       </c>
       <c r="H219" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I219" s="1">
         <v>44851</v>
@@ -9739,7 +9729,7 @@
         <v>44899</v>
       </c>
       <c r="H220" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I220" s="1">
         <v>44860</v>
@@ -9777,7 +9767,7 @@
         <v>44899</v>
       </c>
       <c r="H221" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I221" s="1">
         <v>44866</v>
@@ -9815,7 +9805,7 @@
         <v>44916</v>
       </c>
       <c r="H222" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I222" s="1">
         <v>44866</v>
@@ -9853,7 +9843,7 @@
         <v>44936</v>
       </c>
       <c r="H223" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I223" s="1">
         <v>44867</v>
@@ -9891,7 +9881,7 @@
         <v>44936</v>
       </c>
       <c r="H224" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I224" s="1">
         <v>44881</v>
@@ -9929,7 +9919,7 @@
         <v>44934</v>
       </c>
       <c r="H225" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I225" s="1">
         <v>44884</v>
@@ -9967,7 +9957,7 @@
         <v>44936</v>
       </c>
       <c r="H226" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I226" s="1">
         <v>44891</v>
@@ -10005,7 +9995,7 @@
         <v>44947</v>
       </c>
       <c r="H227" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I227" s="1">
         <v>44896</v>
@@ -10043,7 +10033,7 @@
         <v>44936</v>
       </c>
       <c r="H228" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I228" s="1">
         <v>44896</v>
@@ -10081,7 +10071,7 @@
         <v>44958</v>
       </c>
       <c r="H229" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I229" s="1">
         <v>44896</v>
@@ -10119,7 +10109,7 @@
         <v>44965</v>
       </c>
       <c r="H230" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I230" s="1">
         <v>44914</v>
@@ -10157,7 +10147,7 @@
         <v>44958</v>
       </c>
       <c r="H231" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I231" s="1">
         <v>44910</v>
@@ -10195,7 +10185,7 @@
         <v>44958</v>
       </c>
       <c r="H232" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I232" s="1">
         <v>44923</v>
@@ -10233,7 +10223,7 @@
         <v>44983</v>
       </c>
       <c r="H233" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I233" s="1">
         <v>44927</v>
@@ -10271,7 +10261,7 @@
         <v>44978</v>
       </c>
       <c r="H234" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I234" s="1">
         <v>44927</v>
@@ -10309,7 +10299,7 @@
         <v>44983</v>
       </c>
       <c r="H235" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I235" s="1">
         <v>44926</v>
@@ -10347,7 +10337,7 @@
         <v>44996</v>
       </c>
       <c r="H236" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I236" s="1">
         <v>44945</v>
@@ -10385,7 +10375,7 @@
         <v>44983</v>
       </c>
       <c r="H237" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I237" s="1">
         <v>44943</v>
@@ -10423,7 +10413,7 @@
         <v>45010</v>
       </c>
       <c r="H238" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I238" s="1">
         <v>44953</v>
@@ -10461,7 +10451,7 @@
         <v>45006</v>
       </c>
       <c r="H239" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I239" s="1">
         <v>44958</v>
@@ -10499,7 +10489,7 @@
         <v>45010</v>
       </c>
       <c r="H240" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I240" s="1">
         <v>44958</v>
@@ -10537,7 +10527,7 @@
         <v>45010</v>
       </c>
       <c r="H241" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I241" s="1">
         <v>44956</v>
@@ -10575,7 +10565,7 @@
         <v>45024</v>
       </c>
       <c r="H242" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I242" s="1">
         <v>44976</v>
@@ -10613,7 +10603,7 @@
         <v>45037</v>
       </c>
       <c r="H243" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I243" s="1">
         <v>44972</v>
@@ -10651,7 +10641,7 @@
         <v>45037</v>
       </c>
       <c r="H244" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I244" s="1">
         <v>44981</v>
@@ -10689,7 +10679,7 @@
         <v>45049</v>
       </c>
       <c r="H245" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I245" s="1">
         <v>44986</v>
@@ -10727,7 +10717,7 @@
         <v>45037</v>
       </c>
       <c r="H246" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I246" s="1">
         <v>44986</v>
@@ -10765,7 +10755,7 @@
         <v>45037</v>
       </c>
       <c r="H247" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I247" s="1">
         <v>44986</v>
@@ -10803,7 +10793,7 @@
         <v>45055</v>
       </c>
       <c r="H248" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I248" s="1">
         <v>45004</v>
@@ -10841,7 +10831,7 @@
         <v>45037</v>
       </c>
       <c r="H249" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I249" s="1">
         <v>45002</v>
@@ -10879,7 +10869,7 @@
         <v>45067</v>
       </c>
       <c r="H250" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I250" s="1">
         <v>45013</v>
@@ -10917,7 +10907,7 @@
         <v>45067</v>
       </c>
       <c r="H251" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I251" s="1">
         <v>45017</v>
@@ -10955,7 +10945,7 @@
         <v>45049</v>
       </c>
       <c r="H252" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I252" s="1">
         <v>45017</v>
@@ -10993,7 +10983,7 @@
         <v>45067</v>
       </c>
       <c r="H253" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I253" s="1">
         <v>45017</v>
@@ -11031,7 +11021,7 @@
         <v>45085</v>
       </c>
       <c r="H254" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I254" s="1">
         <v>45035</v>
@@ -11069,7 +11059,7 @@
         <v>45074</v>
       </c>
       <c r="H255" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I255" s="1">
         <v>45034</v>
@@ -11107,7 +11097,7 @@
         <v>45090</v>
       </c>
       <c r="H256" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I256" s="1">
         <v>45042</v>
@@ -11145,7 +11135,7 @@
         <v>45098</v>
       </c>
       <c r="H257" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I257" s="1">
         <v>45047</v>
@@ -11183,7 +11173,7 @@
         <v>45090</v>
       </c>
       <c r="H258" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I258" s="1">
         <v>45047</v>
@@ -11221,7 +11211,7 @@
         <v>45091</v>
       </c>
       <c r="H259" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I259" s="1">
         <v>45048</v>
@@ -11259,7 +11249,7 @@
         <v>45116</v>
       </c>
       <c r="H260" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I260" s="1">
         <v>45065</v>
@@ -11297,7 +11287,7 @@
         <v>45116</v>
       </c>
       <c r="H261" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I261" s="1">
         <v>45065</v>
@@ -11335,7 +11325,7 @@
         <v>45117</v>
       </c>
       <c r="H262" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I262" s="1">
         <v>45072</v>
@@ -11373,7 +11363,7 @@
         <v>45128</v>
       </c>
       <c r="H263" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I263" s="1">
         <v>45078</v>
@@ -11411,7 +11401,7 @@
         <v>45117</v>
       </c>
       <c r="H264" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I264" s="1">
         <v>45078</v>
@@ -11449,7 +11439,7 @@
         <v>45133</v>
       </c>
       <c r="H265" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I265" s="1">
         <v>45077</v>
@@ -11487,7 +11477,7 @@
         <v>45146</v>
       </c>
       <c r="H266" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I266" s="1">
         <v>45096</v>
@@ -11525,7 +11515,7 @@
         <v>45148</v>
       </c>
       <c r="H267" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I267" s="1">
         <v>45096</v>
@@ -11563,7 +11553,7 @@
         <v>45148</v>
       </c>
       <c r="H268" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I268" s="1">
         <v>45105</v>
@@ -11601,7 +11591,7 @@
         <v>45148</v>
       </c>
       <c r="H269" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I269" s="1">
         <v>45108</v>
@@ -11639,7 +11629,7 @@
         <v>45159</v>
       </c>
       <c r="H270" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I270" s="1">
         <v>45108</v>
@@ -11677,7 +11667,7 @@
         <v>45148</v>
       </c>
       <c r="H271" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I271" s="1">
         <v>45107</v>
@@ -11715,7 +11705,7 @@
         <v>45177</v>
       </c>
       <c r="H272" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I272" s="1">
         <v>45126</v>
@@ -11753,7 +11743,7 @@
         <v>45181</v>
       </c>
       <c r="H273" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I273" s="1">
         <v>45126</v>
@@ -11791,7 +11781,7 @@
         <v>45181</v>
       </c>
       <c r="H274" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I274" s="1">
         <v>45134</v>
@@ -11829,7 +11819,7 @@
         <v>45190</v>
       </c>
       <c r="H275" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I275" s="1">
         <v>45139</v>
@@ -11867,7 +11857,7 @@
         <v>45181</v>
       </c>
       <c r="H276" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I276" s="1">
         <v>45139</v>
@@ -11905,7 +11895,7 @@
         <v>45181</v>
       </c>
       <c r="H277" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I277" s="1">
         <v>45138</v>
@@ -11943,7 +11933,7 @@
         <v>45208</v>
       </c>
       <c r="H278" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I278" s="1">
         <v>45157</v>
@@ -11981,7 +11971,7 @@
         <v>45206</v>
       </c>
       <c r="H279" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I279" s="1">
         <v>45156</v>
@@ -12019,7 +12009,7 @@
         <v>45206</v>
       </c>
       <c r="H280" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I280" s="1">
         <v>45167</v>
@@ -12057,7 +12047,7 @@
         <v>45220</v>
       </c>
       <c r="H281" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I281" s="1">
         <v>45170</v>
@@ -12095,7 +12085,7 @@
         <v>45206</v>
       </c>
       <c r="H282" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I282" s="1">
         <v>45170</v>
@@ -12133,7 +12123,7 @@
         <v>45214</v>
       </c>
       <c r="H283" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I283" s="1">
         <v>45169</v>
@@ -12171,7 +12161,7 @@
         <v>45238</v>
       </c>
       <c r="H284" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I284" s="1">
         <v>45188</v>
@@ -12209,7 +12199,7 @@
         <v>45237</v>
       </c>
       <c r="H285" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I285" s="1">
         <v>45184</v>
@@ -12247,7 +12237,7 @@
         <v>45237</v>
       </c>
       <c r="H286" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I286" s="1">
         <v>45196</v>
@@ -12285,7 +12275,7 @@
         <v>45251</v>
       </c>
       <c r="H287" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I287" s="1">
         <v>45200</v>
@@ -12323,7 +12313,7 @@
         <v>45237</v>
       </c>
       <c r="H288" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I288" s="1">
         <v>45200</v>
@@ -12361,7 +12351,7 @@
         <v>45250</v>
       </c>
       <c r="H289" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I289" s="1">
         <v>45201</v>
@@ -12399,7 +12389,7 @@
         <v>45268</v>
       </c>
       <c r="H290" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I290" s="1">
         <v>45218</v>
@@ -12437,7 +12427,7 @@
         <v>45265</v>
       </c>
       <c r="H291" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I291" s="1">
         <v>45217</v>
@@ -12475,7 +12465,7 @@
         <v>45265</v>
       </c>
       <c r="H292" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I292" s="1">
         <v>45225</v>
@@ -12513,7 +12503,7 @@
         <v>45271</v>
       </c>
       <c r="H293" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I293" s="1">
         <v>45231</v>
@@ -12551,7 +12541,7 @@
         <v>45281</v>
       </c>
       <c r="H294" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I294" s="1">
         <v>45231</v>
@@ -12589,7 +12579,7 @@
         <v>45299</v>
       </c>
       <c r="H295" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I295" s="1">
         <v>45232</v>
@@ -12627,7 +12617,7 @@
         <v>45299</v>
       </c>
       <c r="H296" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I296" s="1">
         <v>45249</v>
@@ -12665,7 +12655,7 @@
         <v>45299</v>
       </c>
       <c r="H297" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I297" s="1">
         <v>45250</v>
@@ -12703,7 +12693,7 @@
         <v>45299</v>
       </c>
       <c r="H298" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I298" s="1">
         <v>45258</v>
@@ -12741,7 +12731,7 @@
         <v>45312</v>
       </c>
       <c r="H299" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I299" s="1">
         <v>45261</v>
@@ -12779,7 +12769,7 @@
         <v>45299</v>
       </c>
       <c r="H300" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I300" s="1">
         <v>45261</v>
@@ -12817,7 +12807,7 @@
         <v>45320</v>
       </c>
       <c r="H301" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I301" s="1">
         <v>45262</v>
@@ -12855,7 +12845,7 @@
         <v>45330</v>
       </c>
       <c r="H302" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I302" s="1">
         <v>45279</v>
@@ -12893,7 +12883,7 @@
         <v>45320</v>
       </c>
       <c r="H303" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I303" s="1">
         <v>45278</v>
@@ -12931,7 +12921,7 @@
         <v>45345</v>
       </c>
       <c r="H304" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I304" s="1">
         <v>45287</v>
@@ -12969,7 +12959,7 @@
         <v>45343</v>
       </c>
       <c r="H305" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I305" s="1">
         <v>45292</v>
@@ -13007,7 +12997,7 @@
         <v>45330</v>
       </c>
       <c r="H306" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I306" s="1">
         <v>45292</v>
@@ -13045,7 +13035,7 @@
         <v>45345</v>
       </c>
       <c r="H307" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I307" s="1">
         <v>45294</v>
@@ -13083,7 +13073,7 @@
         <v>45359</v>
       </c>
       <c r="H308" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I308" s="1">
         <v>45310</v>
@@ -13121,7 +13111,7 @@
         <v>45345</v>
       </c>
       <c r="H309" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I309" s="1">
         <v>45310</v>
@@ -13159,7 +13149,7 @@
         <v>45378</v>
       </c>
       <c r="H310" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I310" s="1">
         <v>45318</v>
@@ -13197,7 +13187,7 @@
         <v>45361</v>
       </c>
       <c r="H311" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I311" s="1">
         <v>45323</v>
@@ -13235,7 +13225,7 @@
         <v>45372</v>
       </c>
       <c r="H312" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I312" s="1">
         <v>45323</v>
@@ -13273,7 +13263,7 @@
         <v>45378</v>
       </c>
       <c r="H313" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I313" s="1">
         <v>45323</v>
@@ -13311,7 +13301,7 @@
         <v>45390</v>
       </c>
       <c r="H314" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I314" s="1">
         <v>45341</v>
@@ -13349,7 +13339,7 @@
         <v>45378</v>
       </c>
       <c r="H315" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I315" s="1">
         <v>45338</v>
@@ -13387,7 +13377,7 @@
         <v>45378</v>
       </c>
       <c r="H316" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I316" s="1">
         <v>45349</v>
@@ -13425,7 +13415,7 @@
         <v>45393</v>
       </c>
       <c r="H317" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I317" s="1">
         <v>45352</v>
@@ -13463,7 +13453,7 @@
         <v>45403</v>
       </c>
       <c r="H318" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I318" s="1">
         <v>45352</v>
@@ -13501,7 +13491,7 @@
         <v>45418</v>
       </c>
       <c r="H319" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I319" s="1">
         <v>45355</v>
@@ -13539,7 +13529,7 @@
         <v>45421</v>
       </c>
       <c r="H320" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I320" s="1">
         <v>45370</v>
@@ -13577,7 +13567,7 @@
         <v>45418</v>
       </c>
       <c r="H321" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I321" s="1">
         <v>45369</v>
@@ -13615,7 +13605,7 @@
         <v>45418</v>
       </c>
       <c r="H322" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I322" s="1">
         <v>45377</v>
@@ -13653,7 +13643,7 @@
         <v>45433</v>
       </c>
       <c r="H323" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I323" s="1">
         <v>45383</v>
@@ -13691,7 +13681,7 @@
         <v>45418</v>
       </c>
       <c r="H324" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I324" s="1">
         <v>45383</v>
@@ -13729,7 +13719,7 @@
         <v>45455</v>
       </c>
       <c r="H325" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I325" s="1">
         <v>45385</v>
@@ -13767,7 +13757,7 @@
         <v>45451</v>
       </c>
       <c r="H326" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I326" s="1">
         <v>45401</v>
@@ -13805,7 +13795,7 @@
         <v>45455</v>
       </c>
       <c r="H327" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I327" s="1">
         <v>45400</v>
@@ -13843,7 +13833,7 @@
         <v>45455</v>
       </c>
       <c r="H328" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I328" s="1">
         <v>45408</v>
@@ -13881,7 +13871,7 @@
         <v>45455</v>
       </c>
       <c r="H329" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I329" s="1">
         <v>45413</v>
@@ -13919,7 +13909,7 @@
         <v>45464</v>
       </c>
       <c r="H330" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I330" s="1">
         <v>45413</v>
@@ -13957,7 +13947,7 @@
         <v>45455</v>
       </c>
       <c r="H331" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I331" s="1">
         <v>45415</v>
@@ -13995,7 +13985,7 @@
         <v>45482</v>
       </c>
       <c r="H332" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I332" s="1">
         <v>45431</v>
@@ -14033,7 +14023,7 @@
         <v>45480</v>
       </c>
       <c r="H333" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I333" s="1">
         <v>45429</v>
@@ -14071,7 +14061,7 @@
         <v>45480</v>
       </c>
       <c r="H334" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I334" s="1">
         <v>45440</v>
@@ -14109,7 +14099,7 @@
         <v>45480</v>
       </c>
       <c r="H335" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I335" s="1">
         <v>45444</v>
@@ -14147,7 +14137,7 @@
         <v>45494</v>
       </c>
       <c r="H336" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I336" s="1">
         <v>45444</v>

</xml_diff>

<commit_message>
modified Customer Table to include Firebase login details
</commit_message>
<xml_diff>
--- a/demo_data/demo.xlsx
+++ b/demo_data/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseulloa/Developer/utilities-database-tools/demo_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EB80B7-F132-CF45-AE65-3BF919EBF918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BA9B14-D736-C940-80F7-1922FB7C43B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="840" windowWidth="25800" windowHeight="16940" activeTab="5" xr2:uid="{D5A4ABC1-F07C-5E41-9CF5-2934409BBBCB}"/>
+    <workbookView xWindow="4440" yWindow="840" windowWidth="25800" windowHeight="16940" activeTab="6" xr2:uid="{D5A4ABC1-F07C-5E41-9CF5-2934409BBBCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="6" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Meters" sheetId="5" r:id="rId4"/>
     <sheet name="CustomerProviderUtility" sheetId="7" r:id="rId5"/>
     <sheet name="Bills" sheetId="3" r:id="rId6"/>
+    <sheet name="Postman Test" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,8 +41,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="81">
   <si>
     <t>UtilityID</t>
   </si>
@@ -255,17 +278,54 @@
   <si>
     <t>id</t>
   </si>
+  <si>
+    <t>Add new records</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TableName: </t>
+  </si>
+  <si>
+    <t>Bills</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Set 001</t>
+  </si>
+  <si>
+    <t>Ser 002</t>
+  </si>
+  <si>
+    <t>Unpaid</t>
+  </si>
+  <si>
+    <t>Set 003</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>CustomerProviderUtility</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -277,7 +337,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -285,16 +345,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1190,7 +1544,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E458880D-D775-7B47-83F8-95DB757DD44F}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1367,8 +1723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12801117-A764-174E-AB4F-A29DC92B5033}">
   <dimension ref="A1:L336"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14155,4 +14511,502 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72414C71-F48A-1B49-9FFC-100170FB4298}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="25.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="str">
+        <f>B3</f>
+        <v>Set 001</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:H3" si="0">C3</f>
+        <v>Ser 002</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="0"/>
+        <v>Set 003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="str" cm="1">
+        <f t="array" ref="A4:A12">TRANSPOSE(Bills!B1:J1)</f>
+        <v>CustomerProviderUtilityID</v>
+      </c>
+      <c r="B4" s="7">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="15">
+        <v>4</v>
+      </c>
+      <c r="F4" t="str">
+        <f>"{"""&amp;$A4&amp;""":"""&amp;B4&amp;""","</f>
+        <v>{"CustomerProviderUtilityID":"2",</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" ref="G4:H4" si="1">"{"""&amp;$A4&amp;""":"""&amp;C4&amp;""","</f>
+        <v>{"CustomerProviderUtilityID":"1",</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v>{"CustomerProviderUtilityID":"4",</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="str">
+        <v>IssueDate</v>
+      </c>
+      <c r="B5" s="6">
+        <v>45209</v>
+      </c>
+      <c r="C5" s="6">
+        <v>45483</v>
+      </c>
+      <c r="D5" s="17">
+        <v>45366</v>
+      </c>
+      <c r="F5" t="str">
+        <f>""""&amp;$A5&amp;""":"""&amp;TEXT(B5,"yyyy/mm/dd")&amp;""","</f>
+        <v>"IssueDate":"2023/10/10",</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" ref="G5:H5" si="2">""""&amp;$A5&amp;""":"""&amp;TEXT(C5,"yyyy/mm/dd")&amp;""","</f>
+        <v>"IssueDate":"2024/07/10",</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="2"/>
+        <v>"IssueDate":"2024/03/15",</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="str">
+        <v>AmountBilled</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1500</v>
+      </c>
+      <c r="C6" s="5">
+        <v>4500</v>
+      </c>
+      <c r="D6" s="18">
+        <v>120000</v>
+      </c>
+      <c r="F6" t="str">
+        <f>""""&amp;$A6&amp;""":"""&amp;B6&amp;""","</f>
+        <v>"AmountBilled":"1500",</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" ref="G6:H7" si="3">""""&amp;$A6&amp;""":"""&amp;C6&amp;""","</f>
+        <v>"AmountBilled":"4500",</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="3"/>
+        <v>"AmountBilled":"120000",</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="str">
+        <v>AmountConsumed</v>
+      </c>
+      <c r="B7" s="5">
+        <v>120</v>
+      </c>
+      <c r="C7" s="5">
+        <v>10</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="F7" t="str">
+        <f>""""&amp;$A7&amp;""":"""&amp;IF(ISBLANK(B7),0,B7)&amp;""","</f>
+        <v>"AmountConsumed":"120",</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" ref="G7:H7" si="4">""""&amp;$A7&amp;""":"""&amp;IF(ISBLANK(C7),0,C7)&amp;""","</f>
+        <v>"AmountConsumed":"10",</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="4"/>
+        <v>"AmountConsumed":"0",</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="str">
+        <v>PaymentDeadline</v>
+      </c>
+      <c r="B8" s="6">
+        <v>45245</v>
+      </c>
+      <c r="C8" s="6">
+        <v>45504</v>
+      </c>
+      <c r="D8" s="17">
+        <v>45412</v>
+      </c>
+      <c r="F8" t="str">
+        <f>""""&amp;$A8&amp;""":"""&amp;TEXT(B8,"yyyy/mm/dd")&amp;""","</f>
+        <v>"PaymentDeadline":"2023/11/15",</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" ref="G8:H9" si="5">""""&amp;$A8&amp;""":"""&amp;TEXT(C8,"yyyy/mm/dd")&amp;""","</f>
+        <v>"PaymentDeadline":"2024/07/31",</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="5"/>
+        <v>"PaymentDeadline":"2024/04/30",</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="str">
+        <v>PaymentDate</v>
+      </c>
+      <c r="B9" s="6">
+        <v>45228</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="17">
+        <v>45422</v>
+      </c>
+      <c r="F9" t="str">
+        <f>IF(ISBLANK(B9),"",""""&amp;$A9&amp;""":"""&amp;TEXT(B9,"yyyy/mm/dd")&amp;""",")</f>
+        <v>"PaymentDate":"2023/10/29",</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" ref="G9:H9" si="6">IF(ISBLANK(C9),"",""""&amp;$A9&amp;""":"""&amp;TEXT(C9,"yyyy/mm/dd")&amp;""",")</f>
+        <v/>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="6"/>
+        <v>"PaymentDate":"2024/05/10",</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="str">
+        <v>Status</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="str">
+        <f>""""&amp;$A10&amp;""":"""&amp;B10&amp;""","</f>
+        <v>"Status":"Paid",</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" ref="G10:H10" si="7">""""&amp;$A10&amp;""":"""&amp;C10&amp;""","</f>
+        <v>"Status":"Unpaid",</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="7"/>
+        <v>"Status":"Sumario",</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="str">
+        <v>StartPeriod</v>
+      </c>
+      <c r="B11" s="6">
+        <v>45170</v>
+      </c>
+      <c r="C11" s="6">
+        <v>45444</v>
+      </c>
+      <c r="D11" s="17">
+        <v>45323</v>
+      </c>
+      <c r="F11" t="str">
+        <f>""""&amp;$A11&amp;""":"""&amp;TEXT(B11,"yyyy/mm/dd")&amp;""","</f>
+        <v>"StartPeriod":"2023/09/01",</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" ref="G11:H11" si="8">""""&amp;$A11&amp;""":"""&amp;TEXT(C11,"yyyy/mm/dd")&amp;""","</f>
+        <v>"StartPeriod":"2024/06/01",</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="8"/>
+        <v>"StartPeriod":"2024/02/01",</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="str">
+        <v>EndPeriod</v>
+      </c>
+      <c r="B12" s="20">
+        <v>45199</v>
+      </c>
+      <c r="C12" s="20">
+        <v>45473</v>
+      </c>
+      <c r="D12" s="21">
+        <v>45351</v>
+      </c>
+      <c r="F12" t="str">
+        <f>""""&amp;$A12&amp;""":"""&amp;TEXT(B12,"yyyy/mm/dd")&amp;"""}"</f>
+        <v>"EndPeriod":"2023/09/30"}</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" ref="G12:H12" si="9">""""&amp;$A12&amp;""":"""&amp;TEXT(C12,"yyyy/mm/dd")&amp;"""}"</f>
+        <v>"EndPeriod":"2024/06/30"}</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="9"/>
+        <v>"EndPeriod":"2024/02/29"}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="136" x14ac:dyDescent="0.2">
+      <c r="F13" s="30" t="str">
+        <f>_xlfn.CONCAT(F4:F12)</f>
+        <v>{"CustomerProviderUtilityID":"2","IssueDate":"2023/10/10","AmountBilled":"1500","AmountConsumed":"120","PaymentDeadline":"2023/11/15","PaymentDate":"2023/10/29","Status":"Paid","StartPeriod":"2023/09/01","EndPeriod":"2023/09/30"}</v>
+      </c>
+      <c r="G13" s="30" t="str">
+        <f t="shared" ref="G13:H13" si="10">_xlfn.CONCAT(G4:G12)</f>
+        <v>{"CustomerProviderUtilityID":"1","IssueDate":"2024/07/10","AmountBilled":"4500","AmountConsumed":"10","PaymentDeadline":"2024/07/31","Status":"Unpaid","StartPeriod":"2024/06/01","EndPeriod":"2024/06/30"}</v>
+      </c>
+      <c r="H13" s="30" t="str">
+        <f t="shared" si="10"/>
+        <v>{"CustomerProviderUtilityID":"4","IssueDate":"2024/03/15","AmountBilled":"120000","AmountConsumed":"0","PaymentDeadline":"2024/04/30","PaymentDate":"2024/05/10","Status":"Sumario","StartPeriod":"2024/02/01","EndPeriod":"2024/02/29"}</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+    </row>
+    <row r="16" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" t="str">
+        <f>B16</f>
+        <v>Set 001</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" ref="G16:H16" si="11">C16</f>
+        <v>Ser 002</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="11"/>
+        <v>Set 003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="str" cm="1">
+        <f t="array" ref="A17:A21">TRANSPOSE(CustomerProviderUtility!B1:F1)</f>
+        <v>CustomerID</v>
+      </c>
+      <c r="B17" s="7">
+        <v>1</v>
+      </c>
+      <c r="C17" s="7">
+        <v>1</v>
+      </c>
+      <c r="D17" s="15">
+        <v>1</v>
+      </c>
+      <c r="F17" t="str">
+        <f>"{"""&amp;$A17&amp;""":"""&amp;B17&amp;""","</f>
+        <v>{"CustomerID":"1",</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" ref="G17:H17" si="12">"{"""&amp;$A17&amp;""":"""&amp;C17&amp;""","</f>
+        <v>{"CustomerID":"1",</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="12"/>
+        <v>{"CustomerID":"1",</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="str">
+        <v>ProviderID</v>
+      </c>
+      <c r="B18" s="25">
+        <v>2</v>
+      </c>
+      <c r="C18" s="25">
+        <v>1</v>
+      </c>
+      <c r="D18" s="26">
+        <v>2</v>
+      </c>
+      <c r="F18" t="str">
+        <f>""""&amp;$A18&amp;""":"""&amp;B18&amp;""","</f>
+        <v>"ProviderID":"2",</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" ref="G18:H20" si="13">""""&amp;$A18&amp;""":"""&amp;C18&amp;""","</f>
+        <v>"ProviderID":"1",</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="13"/>
+        <v>"ProviderID":"2",</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="16" t="str">
+        <v>UtilityID</v>
+      </c>
+      <c r="B19" s="5">
+        <v>2</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="18">
+        <v>2</v>
+      </c>
+      <c r="F19" t="str">
+        <f>""""&amp;$A19&amp;""":"""&amp;B19&amp;""","</f>
+        <v>"UtilityID":"2",</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="13"/>
+        <v>"UtilityID":"1",</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="13"/>
+        <v>"UtilityID":"2",</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="16" t="str">
+        <v>MeterID</v>
+      </c>
+      <c r="B20" s="28">
+        <v>4</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="D20" s="18">
+        <v>2</v>
+      </c>
+      <c r="F20" t="str">
+        <f>""""&amp;$A20&amp;""":"""&amp;B20&amp;""","</f>
+        <v>"MeterID":"4",</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="13"/>
+        <v>"MeterID":"1",</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="13"/>
+        <v>"MeterID":"2",</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="str">
+        <v>CustomerNumber</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" t="str">
+        <f>""""&amp;$A21&amp;""":"""&amp;B21&amp;"""}"</f>
+        <v>"CustomerNumber":"Error"}</v>
+      </c>
+      <c r="G21" t="str">
+        <f>""""&amp;$A21&amp;""":"""&amp;C21&amp;"""}"</f>
+        <v>"CustomerNumber":"45023123312"}</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" ref="G21:H21" si="14">""""&amp;$A21&amp;""":"""&amp;D21&amp;"""}"</f>
+        <v>"CustomerNumber":"970190150"}</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="F22" s="30" t="str">
+        <f>_xlfn.CONCAT(F17:F21)</f>
+        <v>{"CustomerID":"1","ProviderID":"2","UtilityID":"2","MeterID":"4","CustomerNumber":"Error"}</v>
+      </c>
+      <c r="G22" s="30" t="str">
+        <f t="shared" ref="G22:H22" si="15">_xlfn.CONCAT(G17:G21)</f>
+        <v>{"CustomerID":"1","ProviderID":"1","UtilityID":"1","MeterID":"1","CustomerNumber":"45023123312"}</v>
+      </c>
+      <c r="H22" s="30" t="str">
+        <f t="shared" si="15"/>
+        <v>{"CustomerID":"1","ProviderID":"2","UtilityID":"2","MeterID":"2","CustomerNumber":"970190150"}</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B15:D15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>